<commit_message>
version 3.2 of TOBI mainboard and associated code -- quick turnaround
</commit_message>
<xml_diff>
--- a/TOBI - BOM.xlsx
+++ b/TOBI - BOM.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danueda/Documents/Grants and Non-Profits/Dynamic Tools/TOBI Resources/finalbomanddriversoftware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcdod\Documents\GitHub\TOBI-Platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="460" windowWidth="23860" windowHeight="15460"/>
+    <workbookView xWindow="1358" yWindow="458" windowWidth="23858" windowHeight="15458"/>
   </bookViews>
   <sheets>
     <sheet name="For robot" sheetId="1" r:id="rId1"/>
     <sheet name="Tools" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="192">
   <si>
     <t>Notes</t>
   </si>
@@ -72,27 +69,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Female Headers 2x2</t>
-  </si>
-  <si>
     <t>Digikey</t>
   </si>
   <si>
-    <t>H2019-ND</t>
-  </si>
-  <si>
-    <t>CONN SOCKET 4POS 2MM DUAL CRIMP</t>
-  </si>
-  <si>
-    <t>Male Headers 2x2</t>
-  </si>
-  <si>
-    <t>H10229-ND</t>
-  </si>
-  <si>
-    <t>CONN HEADER 4POS 2MM PCB TIN</t>
-  </si>
-  <si>
     <t>IO Expander</t>
   </si>
   <si>
@@ -336,12 +315,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=H2019-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/products/en?keywords=H10229-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=CF14JT10K0TR-ND</t>
   </si>
   <si>
@@ -592,6 +565,42 @@
   </si>
   <si>
     <t>Pololu</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/wurth-electronics-inc/61300311121/732-5316-ND/4846825</t>
+  </si>
+  <si>
+    <t>3 pin male header 0.254" pitch</t>
+  </si>
+  <si>
+    <t>2 pin male header 0.254" pitch</t>
+  </si>
+  <si>
+    <t>732-5316-ND</t>
+  </si>
+  <si>
+    <t>3-pin male header</t>
+  </si>
+  <si>
+    <t>2 -pin male header</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/wurth-electronics-inc/61300211121/732-5315-ND/4846823</t>
+  </si>
+  <si>
+    <t>732-5315-ND</t>
+  </si>
+  <si>
+    <t>Jumper wire</t>
+  </si>
+  <si>
+    <t>Female-female jumper wire (20x)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/sparkfun-electronics/PRT-12796/1568-1513-ND/5993861</t>
+  </si>
+  <si>
+    <t>1568-1513-ND</t>
   </si>
 </sst>
 </file>
@@ -818,7 +827,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -931,6 +940,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="30">
     <cellStyle name="Currency" xfId="22" builtinId="4"/>
@@ -969,6 +987,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1271,26 +1292,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="28" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="7"/>
+    <col min="1" max="1" width="18.796875" style="28" customWidth="1"/>
+    <col min="2" max="3" width="8.796875" style="7"/>
     <col min="4" max="4" width="26" style="7" customWidth="1"/>
     <col min="5" max="5" width="30.6640625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="9.86328125" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="7"/>
+    <col min="11" max="16384" width="8.796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1325,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
@@ -1316,16 +1337,16 @@
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -1340,15 +1361,15 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -1359,9 +1380,9 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5" s="10">
         <v>3</v>
@@ -1382,11 +1403,11 @@
         <v>1</v>
       </c>
       <c r="H5" s="49">
-        <f t="shared" ref="H5:H15" si="0">(F5/G5)</f>
+        <f t="shared" ref="H5:H16" si="0">(F5/G5)</f>
         <v>4.25</v>
       </c>
       <c r="I5" s="49">
-        <f t="shared" ref="I5:I15" si="1">(H5*B5)</f>
+        <f t="shared" ref="I5:I16" si="1">(H5*B5)</f>
         <v>12.75</v>
       </c>
       <c r="J5" s="10" t="s">
@@ -1396,534 +1417,546 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="10">
+        <v>6</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="10">
-        <v>12</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="29" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="49">
-        <v>6.86</v>
+        <v>181</v>
+      </c>
+      <c r="F6" s="55">
+        <v>0.64</v>
       </c>
       <c r="G6" s="49">
-        <v>50</v>
-      </c>
-      <c r="H6" s="49">
-        <f t="shared" si="0"/>
-        <v>0.13720000000000002</v>
-      </c>
-      <c r="I6" s="49">
-        <f t="shared" si="1"/>
-        <v>1.6464000000000003</v>
+        <v>0.106</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="55">
+        <v>0.64</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>185</v>
       </c>
       <c r="B7" s="10">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="49">
-        <v>29.9</v>
+        <v>182</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0.64</v>
       </c>
       <c r="G7" s="49">
-        <v>100</v>
-      </c>
-      <c r="H7" s="49">
-        <f t="shared" si="0"/>
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="I7" s="49">
-        <f t="shared" si="1"/>
-        <v>3.5880000000000001</v>
+        <v>0.106</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="55">
+        <v>0.64</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>103</v>
+        <v>186</v>
       </c>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>188</v>
       </c>
       <c r="B8" s="10">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" s="55">
+        <v>3.9</v>
+      </c>
+      <c r="G8" s="49">
+        <v>1.95</v>
+      </c>
+      <c r="H8" s="49"/>
+      <c r="I8" s="55">
+        <v>1.95</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="49">
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="49">
         <v>28.9</v>
       </c>
-      <c r="G8" s="49">
+      <c r="G9" s="49">
         <v>24</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H9" s="49">
         <f t="shared" si="0"/>
         <v>1.2041666666666666</v>
       </c>
-      <c r="I8" s="49">
+      <c r="I9" s="49">
         <f t="shared" si="1"/>
         <v>2.4083333333333332</v>
       </c>
-      <c r="J8" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" s="18">
-        <v>1</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="49">
+      <c r="J9" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="18">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="49">
         <v>0.52</v>
       </c>
-      <c r="G9" s="49">
-        <v>1</v>
-      </c>
-      <c r="H9" s="49">
+      <c r="G10" s="49">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49">
         <f t="shared" si="0"/>
         <v>0.52</v>
       </c>
-      <c r="I9" s="49">
+      <c r="I10" s="49">
         <f t="shared" si="1"/>
         <v>0.52</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="49">
+      <c r="J10" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="49">
         <v>6.37</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G11" s="49">
         <v>12</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H11" s="49">
         <f t="shared" si="0"/>
         <v>0.53083333333333338</v>
       </c>
-      <c r="I10" s="49">
+      <c r="I11" s="49">
         <f t="shared" si="1"/>
         <v>0.53083333333333338</v>
       </c>
-      <c r="J10" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="10">
+      <c r="J11" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="10">
         <v>18</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="49">
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="49">
         <v>23.75</v>
       </c>
-      <c r="G11" s="50">
+      <c r="G12" s="50">
         <v>5000</v>
       </c>
-      <c r="H11" s="49">
+      <c r="H12" s="49">
         <f t="shared" si="0"/>
         <v>4.7499999999999999E-3</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I12" s="49">
         <f t="shared" si="1"/>
         <v>8.5499999999999993E-2</v>
       </c>
-      <c r="J11" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="10">
+      <c r="J12" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="10">
         <v>8</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="49">
+      <c r="C13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="49">
         <v>12.72</v>
       </c>
-      <c r="G12" s="49">
+      <c r="G13" s="49">
         <v>10</v>
       </c>
-      <c r="H12" s="49">
+      <c r="H13" s="49">
         <f t="shared" si="0"/>
         <v>1.272</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I13" s="49">
         <f t="shared" si="1"/>
         <v>10.176</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="10">
-        <v>1</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="49">
+      <c r="J13" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="10">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="49">
         <v>24.95</v>
       </c>
-      <c r="G13" s="49">
-        <v>1</v>
-      </c>
-      <c r="H13" s="49">
+      <c r="G14" s="49">
+        <v>1</v>
+      </c>
+      <c r="H14" s="49">
         <f t="shared" si="0"/>
         <v>24.95</v>
       </c>
-      <c r="I13" s="49">
+      <c r="I14" s="49">
         <f t="shared" si="1"/>
         <v>24.95</v>
       </c>
-      <c r="J13" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="51">
+      <c r="J14" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="14">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="51">
         <v>3.95</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G15" s="51">
         <v>10</v>
       </c>
-      <c r="H14" s="51">
+      <c r="H15" s="51">
         <f t="shared" si="0"/>
         <v>0.39500000000000002</v>
       </c>
-      <c r="I14" s="49">
+      <c r="I15" s="49">
         <f t="shared" si="1"/>
         <v>0.39500000000000002</v>
       </c>
-      <c r="J14" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="14">
-        <v>1</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="51">
+      <c r="J15" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="14">
+        <v>1</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="51">
         <v>1.27</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G16" s="51">
         <v>10</v>
       </c>
-      <c r="H15" s="51">
+      <c r="H16" s="51">
         <f t="shared" si="0"/>
         <v>0.127</v>
       </c>
-      <c r="I15" s="49">
+      <c r="I16" s="49">
         <f t="shared" si="1"/>
         <v>0.127</v>
       </c>
-      <c r="J15" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B16" s="14">
-        <v>1</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="F16" s="51">
+      <c r="J16" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="14">
+        <v>1</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="51">
         <v>0.23</v>
-      </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="14">
-        <v>2</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" s="51">
-        <v>0.25</v>
       </c>
       <c r="G17" s="51"/>
       <c r="H17" s="51"/>
       <c r="I17" s="49"/>
       <c r="J17" s="9" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B18" s="14">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F18" s="51">
-        <v>0.57999999999999996</v>
+        <v>0.25</v>
       </c>
       <c r="G18" s="51"/>
       <c r="H18" s="51"/>
       <c r="I18" s="49"/>
       <c r="J18" s="9" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B19" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="39" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="F19" s="51">
-        <v>2.3199999999999998</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="G19" s="51"/>
       <c r="H19" s="51"/>
       <c r="I19" s="49"/>
       <c r="J19" s="9" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B20" s="14">
         <v>1</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="52">
-        <v>1440</v>
+        <v>14</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>159</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F20" s="51">
-        <v>1.5</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="G20" s="51"/>
       <c r="H20" s="51"/>
       <c r="I20" s="49"/>
       <c r="J20" s="9" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="9"/>
+    <row r="21" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="14">
+        <v>1</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="52">
+        <v>1440</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" s="51">
+        <v>1.5</v>
+      </c>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18">
-        <f>SUM(I5:I15)</f>
-        <v>57.177066666666676</v>
-      </c>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="15"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18">
+        <f>SUM(I5:I16)</f>
+        <v>55.172666666666672</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -1934,7 +1967,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -1945,7 +1978,7 @@
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
@@ -1956,197 +1989,195 @@
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-    </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="10">
-        <v>6</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E30" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="12">
-        <v>22.75</v>
-      </c>
-      <c r="G30" s="10">
-        <v>100</v>
-      </c>
-      <c r="H30" s="10">
-        <f>(F30/G30)</f>
-        <v>0.22750000000000001</v>
-      </c>
-      <c r="I30" s="10">
-        <f>(H30*B30)</f>
-        <v>1.365</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B31" s="10">
         <v>6</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="10">
-        <v>5.4</v>
+        <v>28</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="12">
+        <v>22.75</v>
       </c>
       <c r="G31" s="10">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H31" s="10">
         <f>(F31/G31)</f>
-        <v>5.4</v>
+        <v>0.22750000000000001</v>
       </c>
       <c r="I31" s="10">
         <f>(H31*B31)</f>
-        <v>32.400000000000006</v>
+        <v>1.365</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="K31" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B32" s="10">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" t="s">
-        <v>41</v>
+        <v>9</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" s="12">
-        <v>18.75</v>
+        <v>32</v>
+      </c>
+      <c r="F32" s="10">
+        <v>5.4</v>
       </c>
       <c r="G32" s="10">
-        <v>250</v>
+        <v>1</v>
       </c>
       <c r="H32" s="10">
         <f>(F32/G32)</f>
-        <v>7.4999999999999997E-2</v>
+        <v>5.4</v>
       </c>
       <c r="I32" s="10">
         <f>(H32*B32)</f>
+        <v>32.400000000000006</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="10">
+        <v>30</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="12">
+        <v>18.75</v>
+      </c>
+      <c r="G33" s="10">
+        <v>250</v>
+      </c>
+      <c r="H33" s="10">
+        <f>(F33/G33)</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I33" s="10">
+        <f>(H33*B33)</f>
         <v>2.25</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="K32" s="10"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="32">
-        <v>1</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F33" s="32">
+      <c r="J33" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="32">
+        <v>1</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="32">
         <v>1.5</v>
       </c>
-      <c r="G33" s="32">
+      <c r="G34" s="32">
         <v>50</v>
       </c>
-      <c r="H33" s="22">
-        <f>(F33/G33)</f>
+      <c r="H34" s="22">
+        <f>(F34/G34)</f>
         <v>0.03</v>
       </c>
-      <c r="I33" s="22">
-        <f>(H33*B33)</f>
+      <c r="I34" s="22">
+        <f>(H34*B34)</f>
         <v>0.03</v>
       </c>
-      <c r="J33" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="K33" s="32"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="17">
-        <f>SUM(I30:I32)</f>
+      <c r="J34" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="K34" s="32"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="17">
+        <f>SUM(I31:I33)</f>
         <v>36.015000000000008</v>
       </c>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="23"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20"/>
@@ -2156,374 +2187,384 @@
       <c r="G36" s="20"/>
       <c r="H36" s="24"/>
       <c r="I36" s="20"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="23"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="43"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="9">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+    </row>
+    <row r="40" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="9">
+        <v>6</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="9">
-        <v>1</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-    </row>
-    <row r="39" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B39" s="9">
-        <v>6</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" s="9">
+      <c r="E40" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="9">
         <v>31.16</v>
-      </c>
-      <c r="G39" s="9">
-        <v>10</v>
-      </c>
-      <c r="H39" s="10">
-        <f>(F39/G39)</f>
-        <v>3.1160000000000001</v>
-      </c>
-      <c r="I39" s="10">
-        <f>(H39*B39)</f>
-        <v>18.696000000000002</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="9">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="F40" s="9">
-        <v>0.32</v>
       </c>
       <c r="G40" s="9">
         <v>10</v>
       </c>
       <c r="H40" s="10">
         <f>(F40/G40)</f>
-        <v>3.2000000000000001E-2</v>
+        <v>3.1160000000000001</v>
       </c>
       <c r="I40" s="10">
         <f>(H40*B40)</f>
-        <v>3.2000000000000001E-2</v>
+        <v>18.696000000000002</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="K40" s="9"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>135</v>
+        <v>14</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>129</v>
       </c>
       <c r="F41" s="9">
-        <v>0.89</v>
+        <v>0.32</v>
       </c>
       <c r="G41" s="9">
         <v>10</v>
       </c>
       <c r="H41" s="10">
         <f>(F41/G41)</f>
-        <v>8.8999999999999996E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="I41" s="10">
         <f>(H41*B41)</f>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="K41" s="9"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="9">
+        <v>0.89</v>
+      </c>
+      <c r="G42" s="9">
+        <v>10</v>
+      </c>
+      <c r="H42" s="10">
+        <f>(F42/G42)</f>
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="J41" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="K41" s="9"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="17">
-        <f>SUM(I38:I40)</f>
+      <c r="I42" s="10">
+        <f>(H42*B42)</f>
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="K42" s="9"/>
+    </row>
+    <row r="43" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B43" s="10">
+        <v>6</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="55">
+        <v>0.64</v>
+      </c>
+      <c r="G43" s="49">
+        <v>0.106</v>
+      </c>
+      <c r="H43" s="49"/>
+      <c r="I43" s="55">
+        <v>0.64</v>
+      </c>
+      <c r="J43" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="K43" s="10"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="17">
+        <f>SUM(I39:I41)</f>
         <v>18.728000000000002</v>
       </c>
-      <c r="J42" s="17"/>
-      <c r="K42" s="17"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="23"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="20"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="20"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="42" t="s">
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="23"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="20"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="19"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="24"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+    </row>
+    <row r="48" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="10">
+        <v>1</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="11">
+        <v>36</v>
+      </c>
+      <c r="G48" s="10">
+        <v>1</v>
+      </c>
+      <c r="H48" s="10">
+        <f>(F48/G48)</f>
+        <v>36</v>
+      </c>
+      <c r="I48" s="10">
+        <f>(H48*B48)</f>
+        <v>36</v>
+      </c>
+      <c r="J48" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-    </row>
-    <row r="46" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="10">
-        <v>1</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" s="11">
-        <v>36</v>
-      </c>
-      <c r="G46" s="10">
-        <v>1</v>
-      </c>
-      <c r="H46" s="10">
-        <f>(F46/G46)</f>
-        <v>36</v>
-      </c>
-      <c r="I46" s="10">
-        <f>(H46*B46)</f>
-        <v>36</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K46" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47" s="10">
+      <c r="K48" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="10">
         <v>4</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="E47" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" s="12">
+      <c r="C49" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="12">
         <v>2.2400000000000002</v>
       </c>
-      <c r="G47" s="10">
+      <c r="G49" s="10">
         <v>5</v>
       </c>
-      <c r="H47" s="10">
-        <f>(F47/G47)</f>
+      <c r="H49" s="10">
+        <f>(F49/G49)</f>
         <v>0.44800000000000006</v>
       </c>
-      <c r="I47" s="10">
-        <f>(H47*B47)</f>
+      <c r="I49" s="10">
+        <f>(H49*B49)</f>
         <v>1.7920000000000003</v>
       </c>
-      <c r="J47" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K47" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="17">
-        <f>SUM(I46:I47)</f>
+      <c r="J49" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="17">
+        <f>SUM(I48:I49)</f>
         <v>37.792000000000002</v>
       </c>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
-    </row>
-    <row r="49" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24"/>
-      <c r="K49" s="24"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="19"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="20"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="9"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="9">
-        <v>1</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="9"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+    </row>
+    <row r="51" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="20"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" s="9">
-        <v>6</v>
-      </c>
-      <c r="C53" s="9"/>
+        <v>57</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
+      <c r="E53" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
-      <c r="H53" s="10"/>
+      <c r="H53" s="25"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B54" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -2535,45 +2576,32 @@
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="15" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B55" s="9">
-        <v>1</v>
-      </c>
-      <c r="C55" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E55" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="F55" s="9">
-        <v>5</v>
-      </c>
-      <c r="G55" s="9">
-        <v>1</v>
-      </c>
-      <c r="H55" s="10">
-        <v>5</v>
-      </c>
-      <c r="I55" s="9">
-        <v>5</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>98</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="9"/>
+        <v>60</v>
+      </c>
+      <c r="B56" s="9">
+        <v>6</v>
+      </c>
       <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
@@ -2582,28 +2610,45 @@
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="B57" s="9">
+        <v>1</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E57" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F57" s="9">
+        <v>5</v>
+      </c>
+      <c r="G57" s="9">
+        <v>1</v>
+      </c>
+      <c r="H57" s="10">
+        <v>5</v>
+      </c>
+      <c r="I57" s="9">
+        <v>5</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" s="15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
       <c r="E58" s="9"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -2612,53 +2657,84 @@
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I63" s="7">
-        <f>SUM(I48+I42+I22+I59)</f>
-        <v>113.69706666666667</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="7"/>
-    </row>
-    <row r="65" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A59" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A60" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A62" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A65" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I65" s="7">
+        <f>SUM(I50+I44+I23+I61)</f>
+        <v>111.69266666666667</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="7"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="7"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="7"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="7"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="7"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="7"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A73" s="7"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A74" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" display="http://www.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;itemSeq=222470643&amp;uq=636255435022141425"/>
-    <hyperlink ref="J14" r:id="rId2"/>
+    <hyperlink ref="J15" r:id="rId1"/>
+    <hyperlink ref="J13" r:id="rId2"/>
+    <hyperlink ref="J8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2670,14 +2746,14 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="34" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -2690,9 +2766,9 @@
       <c r="J1" s="35"/>
       <c r="K1" s="35"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -2707,21 +2783,21 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F3" s="9">
         <v>1052.7</v>
@@ -2730,25 +2806,25 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" s="9">
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F4" s="47">
         <v>129</v>
@@ -2759,22 +2835,22 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="11">
@@ -2789,25 +2865,25 @@
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F6" s="9">
         <v>185.98</v>
@@ -2816,19 +2892,19 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B7" s="9">
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -2839,19 +2915,19 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B8" s="9">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F8" s="9">
         <v>10.98</v>
@@ -2862,36 +2938,36 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15.4" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="48" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
@@ -2906,21 +2982,21 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="33" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B11" s="33">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="F11">
         <v>52.05</v>
@@ -2929,24 +3005,24 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="33" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B12" s="33">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F12">
         <v>4.49</v>
@@ -2955,86 +3031,86 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="33" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B14" s="19">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F14" s="53">
         <v>38</v>
       </c>
       <c r="J14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="33" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B15" s="19">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E15" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F15">
         <v>13.08</v>
       </c>
       <c r="J15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="33" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B16" s="19">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F16" s="53">
         <v>5</v>
       </c>
       <c r="J16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="33" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B17" s="19">
         <v>1</v>

</xml_diff>